<commit_message>
- small update to synthesis tracker to include results of TWIST's clonal synthesis run - does not include more detailed order info yet - does not include linear fragments cloned into pSB1C3 by Traci and me/
</commit_message>
<xml_diff>
--- a/2022_release_build_tracker.xlsx
+++ b/2022_release_build_tracker.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B125111-8C79-F545-8363-77E6FD8E42B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED707A5C-5C99-C44F-8F52-51B83770BA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32780" yWindow="-1060" windowWidth="28800" windowHeight="17500" xr2:uid="{A0DFC763-FBFD-2640-B81D-737CE3D1D35E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16000" windowHeight="16000" xr2:uid="{A0DFC763-FBFD-2640-B81D-737CE3D1D35E}"/>
   </bookViews>
   <sheets>
     <sheet name="Build Plan" sheetId="1" r:id="rId1"/>
     <sheet name="Status Terms" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="294">
   <si>
     <t>Part Name</t>
   </si>
@@ -1698,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B7B178-FFA3-1546-B657-00B6ECF2A1CE}">
   <dimension ref="A1:R242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B192" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F208" sqref="F208"/>
+    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1944,7 +1944,9 @@
         <v>1</v>
       </c>
       <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
+      <c r="J12" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
@@ -1970,7 +1972,9 @@
         <v>1</v>
       </c>
       <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
+      <c r="J13" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
       <c r="M13" s="19"/>
@@ -1996,7 +2000,9 @@
         <v>1</v>
       </c>
       <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
+      <c r="J14" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K14" s="19"/>
       <c r="L14" s="19"/>
       <c r="M14" s="19"/>
@@ -2022,7 +2028,9 @@
         <v>1</v>
       </c>
       <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
+      <c r="J15" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
@@ -2048,7 +2056,9 @@
         <v>1</v>
       </c>
       <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
+      <c r="J16" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
@@ -2074,7 +2084,9 @@
         <v>1</v>
       </c>
       <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
+      <c r="J17" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
@@ -2100,7 +2112,9 @@
         <v>1</v>
       </c>
       <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
+      <c r="J18" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K18" s="19"/>
       <c r="L18" s="19"/>
       <c r="M18" s="19"/>
@@ -2126,7 +2140,9 @@
         <v>1</v>
       </c>
       <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
+      <c r="J19" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K19" s="19"/>
       <c r="L19" s="19"/>
       <c r="M19" s="19"/>
@@ -2152,7 +2168,9 @@
         <v>1</v>
       </c>
       <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
+      <c r="J20" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K20" s="19"/>
       <c r="L20" s="19"/>
       <c r="M20" s="19"/>
@@ -2178,7 +2196,9 @@
         <v>1</v>
       </c>
       <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
+      <c r="J21" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K21" s="19"/>
       <c r="L21" s="19"/>
       <c r="M21" s="19"/>
@@ -2204,7 +2224,9 @@
         <v>1</v>
       </c>
       <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
+      <c r="J22" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K22" s="19"/>
       <c r="L22" s="19"/>
       <c r="M22" s="19"/>
@@ -2230,7 +2252,9 @@
         <v>1</v>
       </c>
       <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
+      <c r="J23" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K23" s="19"/>
       <c r="L23" s="19"/>
       <c r="M23" s="19"/>
@@ -2256,7 +2280,9 @@
         <v>1</v>
       </c>
       <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
+      <c r="J24" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
       <c r="M24" s="19"/>
@@ -2282,7 +2308,9 @@
         <v>1</v>
       </c>
       <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
+      <c r="J25" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K25" s="19"/>
       <c r="L25" s="19"/>
       <c r="M25" s="19"/>
@@ -2308,7 +2336,9 @@
         <v>1</v>
       </c>
       <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
+      <c r="J26" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K26" s="19"/>
       <c r="L26" s="19"/>
       <c r="M26" s="19"/>
@@ -2334,7 +2364,9 @@
         <v>1</v>
       </c>
       <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
+      <c r="J27" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K27" s="19"/>
       <c r="L27" s="19"/>
       <c r="M27" s="19"/>
@@ -2360,7 +2392,9 @@
         <v>1</v>
       </c>
       <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="J28" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K28" s="19"/>
       <c r="L28" s="19"/>
       <c r="M28" s="19"/>
@@ -2386,7 +2420,9 @@
         <v>1</v>
       </c>
       <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="J29" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K29" s="19"/>
       <c r="L29" s="19"/>
       <c r="M29" s="19"/>
@@ -2412,7 +2448,9 @@
         <v>1</v>
       </c>
       <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
+      <c r="J30" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K30" s="19"/>
       <c r="L30" s="19"/>
       <c r="M30" s="19"/>
@@ -2438,7 +2476,9 @@
         <v>1</v>
       </c>
       <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
+      <c r="J31" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
       <c r="M31" s="19"/>
@@ -2464,7 +2504,9 @@
         <v>1</v>
       </c>
       <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
+      <c r="J32" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K32" s="19"/>
       <c r="L32" s="19"/>
       <c r="M32" s="19"/>
@@ -2490,7 +2532,9 @@
         <v>1</v>
       </c>
       <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
+      <c r="J33" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K33" s="19"/>
       <c r="L33" s="19"/>
       <c r="M33" s="19"/>
@@ -2516,7 +2560,9 @@
         <v>1</v>
       </c>
       <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
+      <c r="J34" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K34" s="19"/>
       <c r="L34" s="19"/>
       <c r="M34" s="19"/>
@@ -2602,7 +2648,9 @@
         <v>1</v>
       </c>
       <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
+      <c r="J37" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K37" s="19"/>
       <c r="L37" s="19"/>
       <c r="M37" s="19"/>
@@ -2628,7 +2676,9 @@
         <v>1</v>
       </c>
       <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
+      <c r="J38" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K38" s="19"/>
       <c r="L38" s="19"/>
       <c r="M38" s="19"/>
@@ -2880,7 +2930,9 @@
         <v>1</v>
       </c>
       <c r="I47" s="19"/>
-      <c r="J47" s="19"/>
+      <c r="J47" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K47" s="19"/>
       <c r="L47" s="19"/>
       <c r="M47" s="19"/>
@@ -2906,7 +2958,9 @@
         <v>1</v>
       </c>
       <c r="I48" s="19"/>
-      <c r="J48" s="19"/>
+      <c r="J48" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K48" s="19"/>
       <c r="L48" s="19"/>
       <c r="M48" s="19"/>
@@ -2932,7 +2986,9 @@
         <v>1</v>
       </c>
       <c r="I49" s="19"/>
-      <c r="J49" s="19"/>
+      <c r="J49" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K49" s="19"/>
       <c r="L49" s="19"/>
       <c r="M49" s="19"/>
@@ -2986,7 +3042,9 @@
         <v>1</v>
       </c>
       <c r="I51" s="19"/>
-      <c r="J51" s="19"/>
+      <c r="J51" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K51" s="19"/>
       <c r="L51" s="19"/>
       <c r="M51" s="19"/>
@@ -3012,7 +3070,9 @@
         <v>1</v>
       </c>
       <c r="I52" s="19"/>
-      <c r="J52" s="19"/>
+      <c r="J52" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K52" s="19"/>
       <c r="L52" s="19"/>
       <c r="M52" s="19"/>
@@ -3038,7 +3098,9 @@
         <v>1</v>
       </c>
       <c r="I53" s="19"/>
-      <c r="J53" s="19"/>
+      <c r="J53" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K53" s="19"/>
       <c r="L53" s="19"/>
       <c r="M53" s="19"/>
@@ -3092,7 +3154,9 @@
         <v>1</v>
       </c>
       <c r="I55" s="19"/>
-      <c r="J55" s="19"/>
+      <c r="J55" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K55" s="19"/>
       <c r="L55" s="19"/>
       <c r="M55" s="19"/>
@@ -3118,7 +3182,9 @@
         <v>1</v>
       </c>
       <c r="I56" s="19"/>
-      <c r="J56" s="19"/>
+      <c r="J56" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K56" s="19"/>
       <c r="L56" s="19"/>
       <c r="M56" s="19"/>
@@ -3228,7 +3294,9 @@
         <v>1</v>
       </c>
       <c r="I60" s="19"/>
-      <c r="J60" s="19"/>
+      <c r="J60" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K60" s="19"/>
       <c r="L60" s="19"/>
       <c r="M60" s="19"/>
@@ -3254,7 +3322,9 @@
         <v>1</v>
       </c>
       <c r="I61" s="19"/>
-      <c r="J61" s="19"/>
+      <c r="J61" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K61" s="19"/>
       <c r="L61" s="19"/>
       <c r="M61" s="19"/>
@@ -3308,7 +3378,9 @@
         <v>1</v>
       </c>
       <c r="I63" s="19"/>
-      <c r="J63" s="19"/>
+      <c r="J63" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K63" s="19"/>
       <c r="L63" s="19"/>
       <c r="M63" s="19"/>
@@ -3364,7 +3436,9 @@
         <v>1</v>
       </c>
       <c r="I65" s="19"/>
-      <c r="J65" s="19"/>
+      <c r="J65" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K65" s="19"/>
       <c r="L65" s="19"/>
       <c r="M65" s="19"/>
@@ -3418,7 +3492,9 @@
         <v>1</v>
       </c>
       <c r="I67" s="19"/>
-      <c r="J67" s="19"/>
+      <c r="J67" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K67" s="19"/>
       <c r="L67" s="19"/>
       <c r="M67" s="19"/>
@@ -3444,7 +3520,9 @@
         <v>1</v>
       </c>
       <c r="I68" s="19"/>
-      <c r="J68" s="19"/>
+      <c r="J68" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K68" s="19"/>
       <c r="L68" s="19"/>
       <c r="M68" s="19"/>
@@ -3470,7 +3548,9 @@
         <v>1</v>
       </c>
       <c r="I69" s="19"/>
-      <c r="J69" s="19"/>
+      <c r="J69" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K69" s="19"/>
       <c r="L69" s="19"/>
       <c r="M69" s="19"/>
@@ -3524,7 +3604,9 @@
         <v>1</v>
       </c>
       <c r="I71" s="19"/>
-      <c r="J71" s="19"/>
+      <c r="J71" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K71" s="19"/>
       <c r="L71" s="19"/>
       <c r="M71" s="19"/>
@@ -3550,7 +3632,9 @@
         <v>1</v>
       </c>
       <c r="I72" s="19"/>
-      <c r="J72" s="19"/>
+      <c r="J72" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K72" s="19"/>
       <c r="L72" s="19"/>
       <c r="M72" s="19"/>
@@ -3604,7 +3688,9 @@
         <v>1</v>
       </c>
       <c r="I74" s="19"/>
-      <c r="J74" s="19"/>
+      <c r="J74" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K74" s="19"/>
       <c r="L74" s="19"/>
       <c r="M74" s="19"/>
@@ -3686,7 +3772,9 @@
         <v>1</v>
       </c>
       <c r="I77" s="19"/>
-      <c r="J77" s="19"/>
+      <c r="J77" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K77" s="19"/>
       <c r="L77" s="19"/>
       <c r="M77" s="19"/>
@@ -3740,7 +3828,9 @@
         <v>1</v>
       </c>
       <c r="I79" s="19"/>
-      <c r="J79" s="19"/>
+      <c r="J79" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K79" s="19"/>
       <c r="L79" s="19"/>
       <c r="M79" s="19"/>
@@ -3766,7 +3856,9 @@
         <v>1</v>
       </c>
       <c r="I80" s="19"/>
-      <c r="J80" s="19"/>
+      <c r="J80" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K80" s="19"/>
       <c r="L80" s="19"/>
       <c r="M80" s="19"/>
@@ -3792,7 +3884,9 @@
         <v>1</v>
       </c>
       <c r="I81" s="19"/>
-      <c r="J81" s="19"/>
+      <c r="J81" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K81" s="19"/>
       <c r="L81" s="19"/>
       <c r="M81" s="19"/>
@@ -3902,7 +3996,9 @@
         <v>1</v>
       </c>
       <c r="I85" s="19"/>
-      <c r="J85" s="19"/>
+      <c r="J85" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K85" s="19"/>
       <c r="L85" s="19"/>
       <c r="M85" s="19"/>
@@ -3984,7 +4080,9 @@
         <v>1</v>
       </c>
       <c r="I88" s="19"/>
-      <c r="J88" s="19"/>
+      <c r="J88" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K88" s="19"/>
       <c r="L88" s="19"/>
       <c r="M88" s="19"/>
@@ -4010,7 +4108,9 @@
         <v>1</v>
       </c>
       <c r="I89" s="19"/>
-      <c r="J89" s="19"/>
+      <c r="J89" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K89" s="19"/>
       <c r="L89" s="19"/>
       <c r="M89" s="19"/>
@@ -4036,7 +4136,9 @@
         <v>1</v>
       </c>
       <c r="I90" s="19"/>
-      <c r="J90" s="19"/>
+      <c r="J90" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K90" s="19"/>
       <c r="L90" s="19"/>
       <c r="M90" s="19"/>
@@ -4090,7 +4192,9 @@
         <v>1</v>
       </c>
       <c r="I92" s="19"/>
-      <c r="J92" s="19"/>
+      <c r="J92" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K92" s="19"/>
       <c r="L92" s="19"/>
       <c r="M92" s="19"/>
@@ -4144,7 +4248,9 @@
         <v>1</v>
       </c>
       <c r="I94" s="19"/>
-      <c r="J94" s="19"/>
+      <c r="J94" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K94" s="19"/>
       <c r="L94" s="19"/>
       <c r="M94" s="19"/>
@@ -4199,7 +4305,7 @@
       </c>
       <c r="I96" s="19"/>
       <c r="J96" s="19" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="K96" s="19"/>
       <c r="L96" s="19"/>
@@ -4227,7 +4333,7 @@
       </c>
       <c r="I97" s="19"/>
       <c r="J97" s="19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K97" s="19"/>
       <c r="L97" s="19"/>
@@ -4255,7 +4361,7 @@
       </c>
       <c r="I98" s="19"/>
       <c r="J98" s="19" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="K98" s="19"/>
       <c r="L98" s="19"/>
@@ -4283,7 +4389,7 @@
       </c>
       <c r="I99" s="19"/>
       <c r="J99" s="19" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="K99" s="19"/>
       <c r="L99" s="19"/>
@@ -4311,7 +4417,7 @@
       </c>
       <c r="I100" s="19"/>
       <c r="J100" s="19" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="K100" s="19"/>
       <c r="L100" s="19"/>
@@ -4339,7 +4445,7 @@
       </c>
       <c r="I101" s="19"/>
       <c r="J101" s="19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K101" s="19"/>
       <c r="L101" s="19"/>
@@ -4367,7 +4473,7 @@
       </c>
       <c r="I102" s="19"/>
       <c r="J102" s="19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K102" s="19"/>
       <c r="L102" s="19"/>
@@ -4395,7 +4501,7 @@
       </c>
       <c r="I103" s="19"/>
       <c r="J103" s="19" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="K103" s="19"/>
       <c r="L103" s="19"/>
@@ -4423,7 +4529,7 @@
       </c>
       <c r="I104" s="19"/>
       <c r="J104" s="19" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="K104" s="19"/>
       <c r="L104" s="19"/>
@@ -4451,7 +4557,7 @@
       </c>
       <c r="I105" s="19"/>
       <c r="J105" s="19" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="K105" s="19"/>
       <c r="L105" s="19"/>
@@ -4479,7 +4585,7 @@
       </c>
       <c r="I106" s="19"/>
       <c r="J106" s="19" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="K106" s="19"/>
       <c r="L106" s="19"/>
@@ -4507,7 +4613,7 @@
       </c>
       <c r="I107" s="19"/>
       <c r="J107" s="19" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="K107" s="19"/>
       <c r="L107" s="19"/>
@@ -4535,7 +4641,7 @@
       </c>
       <c r="I108" s="19"/>
       <c r="J108" s="19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K108" s="19"/>
       <c r="L108" s="19"/>
@@ -4563,7 +4669,7 @@
       </c>
       <c r="I109" s="19"/>
       <c r="J109" s="19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K109" s="19"/>
       <c r="L109" s="19"/>
@@ -4618,7 +4724,9 @@
         <v>1</v>
       </c>
       <c r="I111" s="19"/>
-      <c r="J111" s="19"/>
+      <c r="J111" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K111" s="19"/>
       <c r="L111" s="19"/>
       <c r="M111" s="19"/>
@@ -4644,7 +4752,9 @@
         <v>1</v>
       </c>
       <c r="I112" s="19"/>
-      <c r="J112" s="19"/>
+      <c r="J112" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K112" s="19"/>
       <c r="L112" s="19"/>
       <c r="M112" s="19"/>
@@ -4670,7 +4780,9 @@
         <v>1</v>
       </c>
       <c r="I113" s="19"/>
-      <c r="J113" s="19"/>
+      <c r="J113" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K113" s="19"/>
       <c r="L113" s="19"/>
       <c r="M113" s="19"/>
@@ -4696,7 +4808,9 @@
         <v>1</v>
       </c>
       <c r="I114" s="19"/>
-      <c r="J114" s="19"/>
+      <c r="J114" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K114" s="19"/>
       <c r="L114" s="19"/>
       <c r="M114" s="19"/>
@@ -4722,7 +4836,9 @@
         <v>1</v>
       </c>
       <c r="I115" s="19"/>
-      <c r="J115" s="19"/>
+      <c r="J115" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K115" s="19"/>
       <c r="L115" s="19"/>
       <c r="M115" s="19"/>
@@ -4748,7 +4864,9 @@
         <v>1</v>
       </c>
       <c r="I116" s="19"/>
-      <c r="J116" s="19"/>
+      <c r="J116" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K116" s="19"/>
       <c r="L116" s="19"/>
       <c r="M116" s="19"/>
@@ -4774,7 +4892,9 @@
         <v>1</v>
       </c>
       <c r="I117" s="19"/>
-      <c r="J117" s="19"/>
+      <c r="J117" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K117" s="19"/>
       <c r="L117" s="19"/>
       <c r="M117" s="19"/>
@@ -4800,7 +4920,9 @@
         <v>1</v>
       </c>
       <c r="I118" s="19"/>
-      <c r="J118" s="19"/>
+      <c r="J118" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K118" s="19"/>
       <c r="L118" s="19"/>
       <c r="M118" s="19"/>
@@ -4826,7 +4948,9 @@
         <v>1</v>
       </c>
       <c r="I119" s="19"/>
-      <c r="J119" s="19"/>
+      <c r="J119" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K119" s="19"/>
       <c r="L119" s="19"/>
       <c r="M119" s="19"/>
@@ -4852,7 +4976,9 @@
         <v>1</v>
       </c>
       <c r="I120" s="19"/>
-      <c r="J120" s="19"/>
+      <c r="J120" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K120" s="19"/>
       <c r="L120" s="19"/>
       <c r="M120" s="19"/>
@@ -4878,7 +5004,9 @@
         <v>1</v>
       </c>
       <c r="I121" s="19"/>
-      <c r="J121" s="19"/>
+      <c r="J121" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K121" s="19"/>
       <c r="L121" s="19"/>
       <c r="M121" s="19"/>
@@ -4964,7 +5092,9 @@
         <v>1</v>
       </c>
       <c r="I124" s="19"/>
-      <c r="J124" s="19"/>
+      <c r="J124" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K124" s="19"/>
       <c r="L124" s="19"/>
       <c r="M124" s="19"/>
@@ -4990,7 +5120,9 @@
         <v>1</v>
       </c>
       <c r="I125" s="19"/>
-      <c r="J125" s="19"/>
+      <c r="J125" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K125" s="19"/>
       <c r="L125" s="19"/>
       <c r="M125" s="19"/>
@@ -5016,7 +5148,9 @@
         <v>1</v>
       </c>
       <c r="I126" s="19"/>
-      <c r="J126" s="19"/>
+      <c r="J126" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K126" s="19"/>
       <c r="L126" s="19"/>
       <c r="M126" s="19"/>
@@ -5042,7 +5176,9 @@
         <v>1</v>
       </c>
       <c r="I127" s="19"/>
-      <c r="J127" s="19"/>
+      <c r="J127" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K127" s="19"/>
       <c r="L127" s="19"/>
       <c r="M127" s="19"/>
@@ -5068,7 +5204,9 @@
         <v>1</v>
       </c>
       <c r="I128" s="19"/>
-      <c r="J128" s="19"/>
+      <c r="J128" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K128" s="19"/>
       <c r="L128" s="19"/>
       <c r="M128" s="19"/>
@@ -5094,7 +5232,9 @@
         <v>1</v>
       </c>
       <c r="I129" s="19"/>
-      <c r="J129" s="19"/>
+      <c r="J129" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K129" s="19"/>
       <c r="L129" s="19"/>
       <c r="M129" s="19"/>
@@ -5120,7 +5260,9 @@
         <v>1</v>
       </c>
       <c r="I130" s="19"/>
-      <c r="J130" s="19"/>
+      <c r="J130" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K130" s="19"/>
       <c r="L130" s="19"/>
       <c r="M130" s="19"/>
@@ -5146,7 +5288,9 @@
         <v>1</v>
       </c>
       <c r="I131" s="19"/>
-      <c r="J131" s="19"/>
+      <c r="J131" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K131" s="19"/>
       <c r="L131" s="19"/>
       <c r="M131" s="19"/>
@@ -5172,7 +5316,9 @@
         <v>1</v>
       </c>
       <c r="I132" s="19"/>
-      <c r="J132" s="19"/>
+      <c r="J132" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K132" s="19"/>
       <c r="L132" s="19"/>
       <c r="M132" s="19"/>
@@ -5198,7 +5344,9 @@
         <v>1</v>
       </c>
       <c r="I133" s="19"/>
-      <c r="J133" s="19"/>
+      <c r="J133" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K133" s="19"/>
       <c r="L133" s="19"/>
       <c r="M133" s="19"/>
@@ -5252,7 +5400,9 @@
         <v>1</v>
       </c>
       <c r="I135" s="19"/>
-      <c r="J135" s="19"/>
+      <c r="J135" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K135" s="19"/>
       <c r="L135" s="19"/>
       <c r="M135" s="19"/>
@@ -5306,7 +5456,9 @@
         <v>1</v>
       </c>
       <c r="I137" s="19"/>
-      <c r="J137" s="19"/>
+      <c r="J137" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K137" s="19"/>
       <c r="L137" s="19"/>
       <c r="M137" s="19"/>
@@ -5332,7 +5484,9 @@
         <v>1</v>
       </c>
       <c r="I138" s="19"/>
-      <c r="J138" s="19"/>
+      <c r="J138" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K138" s="19"/>
       <c r="L138" s="19"/>
       <c r="M138" s="19"/>
@@ -5414,7 +5568,9 @@
         <v>1</v>
       </c>
       <c r="I141" s="19"/>
-      <c r="J141" s="19"/>
+      <c r="J141" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K141" s="19"/>
       <c r="L141" s="19"/>
       <c r="M141" s="19"/>
@@ -5440,7 +5596,9 @@
         <v>1</v>
       </c>
       <c r="I142" s="19"/>
-      <c r="J142" s="19"/>
+      <c r="J142" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K142" s="19"/>
       <c r="L142" s="19"/>
       <c r="M142" s="19"/>
@@ -5496,7 +5654,9 @@
         <v>1</v>
       </c>
       <c r="I144" s="19"/>
-      <c r="J144" s="19"/>
+      <c r="J144" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K144" s="19"/>
       <c r="L144" s="19"/>
       <c r="M144" s="19"/>
@@ -5522,7 +5682,9 @@
         <v>1</v>
       </c>
       <c r="I145" s="19"/>
-      <c r="J145" s="19"/>
+      <c r="J145" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K145" s="19"/>
       <c r="L145" s="19"/>
       <c r="M145" s="19"/>
@@ -5548,7 +5710,9 @@
         <v>1</v>
       </c>
       <c r="I146" s="19"/>
-      <c r="J146" s="19"/>
+      <c r="J146" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K146" s="19"/>
       <c r="L146" s="19"/>
       <c r="M146" s="19"/>
@@ -5574,7 +5738,9 @@
         <v>1</v>
       </c>
       <c r="I147" s="19"/>
-      <c r="J147" s="19"/>
+      <c r="J147" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K147" s="19"/>
       <c r="L147" s="19"/>
       <c r="M147" s="19"/>
@@ -5600,7 +5766,9 @@
         <v>1</v>
       </c>
       <c r="I148" s="19"/>
-      <c r="J148" s="19"/>
+      <c r="J148" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K148" s="19"/>
       <c r="L148" s="19"/>
       <c r="M148" s="19"/>
@@ -5626,7 +5794,9 @@
         <v>1</v>
       </c>
       <c r="I149" s="19"/>
-      <c r="J149" s="19"/>
+      <c r="J149" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K149" s="19"/>
       <c r="L149" s="19"/>
       <c r="M149" s="19"/>
@@ -5652,7 +5822,9 @@
         <v>1</v>
       </c>
       <c r="I150" s="19"/>
-      <c r="J150" s="19"/>
+      <c r="J150" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K150" s="19"/>
       <c r="L150" s="19"/>
       <c r="M150" s="19"/>
@@ -5678,7 +5850,9 @@
         <v>1</v>
       </c>
       <c r="I151" s="19"/>
-      <c r="J151" s="19"/>
+      <c r="J151" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K151" s="19"/>
       <c r="L151" s="19"/>
       <c r="M151" s="19"/>
@@ -5704,7 +5878,9 @@
         <v>1</v>
       </c>
       <c r="I152" s="19"/>
-      <c r="J152" s="19"/>
+      <c r="J152" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K152" s="19"/>
       <c r="L152" s="19"/>
       <c r="M152" s="19"/>
@@ -5730,7 +5906,9 @@
         <v>1</v>
       </c>
       <c r="I153" s="19"/>
-      <c r="J153" s="19"/>
+      <c r="J153" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K153" s="19"/>
       <c r="L153" s="19"/>
       <c r="M153" s="19"/>
@@ -5756,7 +5934,9 @@
         <v>1</v>
       </c>
       <c r="I154" s="19"/>
-      <c r="J154" s="19"/>
+      <c r="J154" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K154" s="19"/>
       <c r="L154" s="19"/>
       <c r="M154" s="19"/>
@@ -5782,7 +5962,9 @@
         <v>1</v>
       </c>
       <c r="I155" s="19"/>
-      <c r="J155" s="19"/>
+      <c r="J155" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K155" s="19"/>
       <c r="L155" s="19"/>
       <c r="M155" s="19"/>
@@ -5836,7 +6018,9 @@
         <v>1</v>
       </c>
       <c r="I157" s="19"/>
-      <c r="J157" s="19"/>
+      <c r="J157" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K157" s="19"/>
       <c r="L157" s="19"/>
       <c r="M157" s="19"/>
@@ -5862,7 +6046,9 @@
         <v>1</v>
       </c>
       <c r="I158" s="19"/>
-      <c r="J158" s="19"/>
+      <c r="J158" s="19" t="s">
+        <v>15</v>
+      </c>
       <c r="K158" s="19"/>
       <c r="L158" s="19"/>
       <c r="M158" s="19"/>
@@ -5888,7 +6074,9 @@
         <v>1</v>
       </c>
       <c r="I159" s="19"/>
-      <c r="J159" s="19"/>
+      <c r="J159" s="19" t="s">
+        <v>15</v>
+      </c>
       <c r="K159" s="19"/>
       <c r="L159" s="19"/>
       <c r="M159" s="19"/>
@@ -5942,7 +6130,9 @@
         <v>1</v>
       </c>
       <c r="I161" s="19"/>
-      <c r="J161" s="19"/>
+      <c r="J161" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K161" s="19"/>
       <c r="L161" s="19"/>
       <c r="M161" s="19"/>
@@ -5968,7 +6158,9 @@
         <v>1</v>
       </c>
       <c r="I162" s="19"/>
-      <c r="J162" s="19"/>
+      <c r="J162" s="19" t="s">
+        <v>15</v>
+      </c>
       <c r="K162" s="19"/>
       <c r="L162" s="19"/>
       <c r="M162" s="19"/>
@@ -5994,7 +6186,9 @@
         <v>1</v>
       </c>
       <c r="I163" s="19"/>
-      <c r="J163" s="19"/>
+      <c r="J163" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K163" s="19"/>
       <c r="L163" s="19"/>
       <c r="M163" s="19"/>
@@ -6020,7 +6214,9 @@
         <v>1</v>
       </c>
       <c r="I164" s="19"/>
-      <c r="J164" s="19"/>
+      <c r="J164" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K164" s="19"/>
       <c r="L164" s="19"/>
       <c r="M164" s="19"/>
@@ -6046,7 +6242,9 @@
         <v>1</v>
       </c>
       <c r="I165" s="19"/>
-      <c r="J165" s="19"/>
+      <c r="J165" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K165" s="19"/>
       <c r="L165" s="19"/>
       <c r="M165" s="19"/>
@@ -6072,7 +6270,9 @@
         <v>1</v>
       </c>
       <c r="I166" s="19"/>
-      <c r="J166" s="19"/>
+      <c r="J166" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K166" s="19"/>
       <c r="L166" s="19"/>
       <c r="M166" s="19"/>
@@ -6098,7 +6298,9 @@
         <v>1</v>
       </c>
       <c r="I167" s="19"/>
-      <c r="J167" s="19"/>
+      <c r="J167" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K167" s="19"/>
       <c r="L167" s="19"/>
       <c r="M167" s="19"/>
@@ -6124,7 +6326,9 @@
         <v>1</v>
       </c>
       <c r="I168" s="19"/>
-      <c r="J168" s="19"/>
+      <c r="J168" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K168" s="19"/>
       <c r="L168" s="19"/>
       <c r="M168" s="19"/>
@@ -6208,7 +6412,9 @@
         <v>1</v>
       </c>
       <c r="I171" s="19"/>
-      <c r="J171" s="19"/>
+      <c r="J171" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K171" s="19"/>
       <c r="L171" s="19"/>
       <c r="M171" s="19"/>
@@ -6234,7 +6440,9 @@
         <v>1</v>
       </c>
       <c r="I172" s="19"/>
-      <c r="J172" s="19"/>
+      <c r="J172" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K172" s="19"/>
       <c r="L172" s="19"/>
       <c r="M172" s="19"/>
@@ -6260,7 +6468,9 @@
         <v>1</v>
       </c>
       <c r="I173" s="19"/>
-      <c r="J173" s="19"/>
+      <c r="J173" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K173" s="19"/>
       <c r="L173" s="19"/>
       <c r="M173" s="19"/>
@@ -6314,7 +6524,9 @@
         <v>1</v>
       </c>
       <c r="I175" s="19"/>
-      <c r="J175" s="19"/>
+      <c r="J175" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K175" s="19"/>
       <c r="L175" s="19"/>
       <c r="M175" s="19"/>
@@ -6370,7 +6582,9 @@
         <v>1</v>
       </c>
       <c r="I177" s="19"/>
-      <c r="J177" s="19"/>
+      <c r="J177" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K177" s="19"/>
       <c r="L177" s="19"/>
       <c r="M177" s="19"/>
@@ -6396,7 +6610,9 @@
         <v>1</v>
       </c>
       <c r="I178" s="19"/>
-      <c r="J178" s="19"/>
+      <c r="J178" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K178" s="19"/>
       <c r="L178" s="19"/>
       <c r="M178" s="19"/>
@@ -6452,7 +6668,9 @@
         <v>1</v>
       </c>
       <c r="I180" s="19"/>
-      <c r="J180" s="19"/>
+      <c r="J180" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K180" s="19"/>
       <c r="L180" s="19"/>
       <c r="M180" s="19"/>
@@ -6508,7 +6726,9 @@
         <v>1</v>
       </c>
       <c r="I182" s="19"/>
-      <c r="J182" s="19"/>
+      <c r="J182" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K182" s="19"/>
       <c r="L182" s="19"/>
       <c r="M182" s="19"/>
@@ -6562,7 +6782,9 @@
         <v>1</v>
       </c>
       <c r="I184" s="19"/>
-      <c r="J184" s="19"/>
+      <c r="J184" s="19" t="s">
+        <v>15</v>
+      </c>
       <c r="K184" s="19"/>
       <c r="L184" s="19"/>
       <c r="M184" s="19"/>
@@ -6618,7 +6840,9 @@
         <v>1</v>
       </c>
       <c r="I186" s="19"/>
-      <c r="J186" s="19"/>
+      <c r="J186" s="19" t="s">
+        <v>15</v>
+      </c>
       <c r="K186" s="19"/>
       <c r="L186" s="19"/>
       <c r="M186" s="19"/>
@@ -6672,7 +6896,9 @@
         <v>1</v>
       </c>
       <c r="I188" s="19"/>
-      <c r="J188" s="19"/>
+      <c r="J188" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K188" s="19"/>
       <c r="L188" s="19"/>
       <c r="M188" s="19"/>
@@ -6698,7 +6924,9 @@
         <v>1</v>
       </c>
       <c r="I189" s="19"/>
-      <c r="J189" s="19"/>
+      <c r="J189" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K189" s="19"/>
       <c r="L189" s="19"/>
       <c r="M189" s="19"/>
@@ -6724,7 +6952,9 @@
         <v>1</v>
       </c>
       <c r="I190" s="19"/>
-      <c r="J190" s="19"/>
+      <c r="J190" s="19" t="s">
+        <v>15</v>
+      </c>
       <c r="K190" s="19"/>
       <c r="L190" s="19"/>
       <c r="M190" s="19"/>
@@ -6750,7 +6980,9 @@
         <v>1</v>
       </c>
       <c r="I191" s="19"/>
-      <c r="J191" s="19"/>
+      <c r="J191" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K191" s="19"/>
       <c r="L191" s="19"/>
       <c r="M191" s="19"/>
@@ -6776,7 +7008,9 @@
         <v>1</v>
       </c>
       <c r="I192" s="19"/>
-      <c r="J192" s="19"/>
+      <c r="J192" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K192" s="19"/>
       <c r="L192" s="19"/>
       <c r="M192" s="19"/>
@@ -6802,7 +7036,9 @@
         <v>1</v>
       </c>
       <c r="I193" s="19"/>
-      <c r="J193" s="19"/>
+      <c r="J193" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K193" s="19"/>
       <c r="L193" s="19"/>
       <c r="M193" s="19"/>
@@ -6888,7 +7124,9 @@
         <v>1</v>
       </c>
       <c r="I196" s="19"/>
-      <c r="J196" s="19"/>
+      <c r="J196" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K196" s="19"/>
       <c r="L196" s="19"/>
       <c r="M196" s="19"/>
@@ -6914,7 +7152,9 @@
         <v>1</v>
       </c>
       <c r="I197" s="19"/>
-      <c r="J197" s="19"/>
+      <c r="J197" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K197" s="19"/>
       <c r="L197" s="19"/>
       <c r="M197" s="19"/>
@@ -7166,7 +7406,9 @@
         <v>1</v>
       </c>
       <c r="I206" s="19"/>
-      <c r="J206" s="19"/>
+      <c r="J206" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K206" s="19"/>
       <c r="L206" s="19"/>
       <c r="M206" s="19"/>
@@ -7192,7 +7434,9 @@
         <v>1</v>
       </c>
       <c r="I207" s="19"/>
-      <c r="J207" s="19"/>
+      <c r="J207" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K207" s="19"/>
       <c r="L207" s="19"/>
       <c r="M207" s="19"/>
@@ -7218,7 +7462,9 @@
         <v>1</v>
       </c>
       <c r="I208" s="19"/>
-      <c r="J208" s="19"/>
+      <c r="J208" s="19" t="s">
+        <v>15</v>
+      </c>
       <c r="K208" s="19"/>
       <c r="L208" s="19"/>
       <c r="M208" s="19"/>
@@ -7244,7 +7490,9 @@
         <v>1</v>
       </c>
       <c r="I209" s="19"/>
-      <c r="J209" s="19"/>
+      <c r="J209" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K209" s="19"/>
       <c r="L209" s="19"/>
       <c r="M209" s="19"/>
@@ -7270,7 +7518,9 @@
         <v>1</v>
       </c>
       <c r="I210" s="19"/>
-      <c r="J210" s="19"/>
+      <c r="J210" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K210" s="19"/>
       <c r="L210" s="19"/>
       <c r="M210" s="19"/>
@@ -7296,7 +7546,9 @@
         <v>1</v>
       </c>
       <c r="I211" s="19"/>
-      <c r="J211" s="19"/>
+      <c r="J211" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K211" s="19"/>
       <c r="L211" s="19"/>
       <c r="M211" s="19"/>
@@ -7322,7 +7574,9 @@
         <v>1</v>
       </c>
       <c r="I212" s="19"/>
-      <c r="J212" s="19"/>
+      <c r="J212" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K212" s="19"/>
       <c r="L212" s="19"/>
       <c r="M212" s="19"/>
@@ -7348,7 +7602,9 @@
         <v>1</v>
       </c>
       <c r="I213" s="19"/>
-      <c r="J213" s="19"/>
+      <c r="J213" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K213" s="19"/>
       <c r="L213" s="19"/>
       <c r="M213" s="19"/>
@@ -7374,7 +7630,9 @@
         <v>1</v>
       </c>
       <c r="I214" s="19"/>
-      <c r="J214" s="19"/>
+      <c r="J214" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K214" s="19"/>
       <c r="L214" s="19"/>
       <c r="M214" s="19"/>
@@ -7400,7 +7658,9 @@
         <v>1</v>
       </c>
       <c r="I215" s="19"/>
-      <c r="J215" s="19"/>
+      <c r="J215" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K215" s="19"/>
       <c r="L215" s="19"/>
       <c r="M215" s="19"/>
@@ -7456,7 +7716,9 @@
         <v>1</v>
       </c>
       <c r="I217" s="19"/>
-      <c r="J217" s="19"/>
+      <c r="J217" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K217" s="19"/>
       <c r="L217" s="19"/>
       <c r="M217" s="19"/>
@@ -7482,7 +7744,9 @@
         <v>1</v>
       </c>
       <c r="I218" s="19"/>
-      <c r="J218" s="19"/>
+      <c r="J218" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K218" s="19"/>
       <c r="L218" s="19"/>
       <c r="M218" s="19"/>
@@ -7508,7 +7772,9 @@
         <v>1</v>
       </c>
       <c r="I219" s="19"/>
-      <c r="J219" s="19"/>
+      <c r="J219" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K219" s="19"/>
       <c r="L219" s="19"/>
       <c r="M219" s="19"/>
@@ -7534,7 +7800,9 @@
         <v>1</v>
       </c>
       <c r="I220" s="19"/>
-      <c r="J220" s="19"/>
+      <c r="J220" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K220" s="19"/>
       <c r="L220" s="19"/>
       <c r="M220" s="19"/>
@@ -7560,7 +7828,9 @@
         <v>1</v>
       </c>
       <c r="I221" s="19"/>
-      <c r="J221" s="19"/>
+      <c r="J221" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K221" s="19"/>
       <c r="L221" s="19"/>
       <c r="M221" s="19"/>
@@ -7586,7 +7856,9 @@
         <v>1</v>
       </c>
       <c r="I222" s="19"/>
-      <c r="J222" s="19"/>
+      <c r="J222" s="19" t="s">
+        <v>15</v>
+      </c>
       <c r="K222" s="19"/>
       <c r="L222" s="19"/>
       <c r="M222" s="19"/>
@@ -7612,7 +7884,9 @@
         <v>1</v>
       </c>
       <c r="I223" s="19"/>
-      <c r="J223" s="19"/>
+      <c r="J223" s="19" t="s">
+        <v>15</v>
+      </c>
       <c r="K223" s="19"/>
       <c r="L223" s="19"/>
       <c r="M223" s="19"/>
@@ -7638,7 +7912,9 @@
         <v>1</v>
       </c>
       <c r="I224" s="19"/>
-      <c r="J224" s="19"/>
+      <c r="J224" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K224" s="19"/>
       <c r="L224" s="19"/>
       <c r="M224" s="19"/>
@@ -7664,7 +7940,9 @@
         <v>1</v>
       </c>
       <c r="I225" s="19"/>
-      <c r="J225" s="19"/>
+      <c r="J225" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K225" s="19"/>
       <c r="L225" s="19"/>
       <c r="M225" s="19"/>
@@ -7690,7 +7968,9 @@
         <v>1</v>
       </c>
       <c r="I226" s="19"/>
-      <c r="J226" s="19"/>
+      <c r="J226" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K226" s="19"/>
       <c r="L226" s="19"/>
       <c r="M226" s="19"/>
@@ -7716,7 +7996,9 @@
         <v>1</v>
       </c>
       <c r="I227" s="19"/>
-      <c r="J227" s="19"/>
+      <c r="J227" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K227" s="19"/>
       <c r="L227" s="19"/>
       <c r="M227" s="19"/>
@@ -7742,7 +8024,9 @@
         <v>1</v>
       </c>
       <c r="I228" s="19"/>
-      <c r="J228" s="19"/>
+      <c r="J228" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K228" s="19"/>
       <c r="L228" s="19"/>
       <c r="M228" s="19"/>
@@ -7768,7 +8052,9 @@
         <v>1</v>
       </c>
       <c r="I229" s="19"/>
-      <c r="J229" s="19"/>
+      <c r="J229" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K229" s="19"/>
       <c r="L229" s="19"/>
       <c r="M229" s="19"/>
@@ -7794,7 +8080,9 @@
         <v>1</v>
       </c>
       <c r="I230" s="19"/>
-      <c r="J230" s="19"/>
+      <c r="J230" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K230" s="19"/>
       <c r="L230" s="19"/>
       <c r="M230" s="19"/>
@@ -7820,7 +8108,9 @@
         <v>1</v>
       </c>
       <c r="I231" s="19"/>
-      <c r="J231" s="19"/>
+      <c r="J231" s="19" t="s">
+        <v>15</v>
+      </c>
       <c r="K231" s="19"/>
       <c r="L231" s="19"/>
       <c r="M231" s="19"/>
@@ -7846,7 +8136,9 @@
         <v>1</v>
       </c>
       <c r="I232" s="19"/>
-      <c r="J232" s="19"/>
+      <c r="J232" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K232" s="19"/>
       <c r="L232" s="19"/>
       <c r="M232" s="19"/>
@@ -7872,7 +8164,9 @@
         <v>1</v>
       </c>
       <c r="I233" s="19"/>
-      <c r="J233" s="19"/>
+      <c r="J233" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K233" s="19"/>
       <c r="L233" s="19"/>
       <c r="M233" s="19"/>
@@ -7898,7 +8192,9 @@
         <v>1</v>
       </c>
       <c r="I234" s="19"/>
-      <c r="J234" s="19"/>
+      <c r="J234" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K234" s="19"/>
       <c r="L234" s="19"/>
       <c r="M234" s="19"/>
@@ -7924,7 +8220,9 @@
         <v>1</v>
       </c>
       <c r="I235" s="19"/>
-      <c r="J235" s="19"/>
+      <c r="J235" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K235" s="19"/>
       <c r="L235" s="19"/>
       <c r="M235" s="19"/>
@@ -7950,7 +8248,9 @@
         <v>1</v>
       </c>
       <c r="I236" s="19"/>
-      <c r="J236" s="19"/>
+      <c r="J236" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K236" s="19"/>
       <c r="L236" s="19"/>
       <c r="M236" s="19"/>
@@ -7976,7 +8276,9 @@
         <v>1</v>
       </c>
       <c r="I237" s="19"/>
-      <c r="J237" s="19"/>
+      <c r="J237" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K237" s="19"/>
       <c r="L237" s="19"/>
       <c r="M237" s="19"/>
@@ -8002,7 +8304,9 @@
         <v>1</v>
       </c>
       <c r="I238" s="19"/>
-      <c r="J238" s="19"/>
+      <c r="J238" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K238" s="19"/>
       <c r="L238" s="19"/>
       <c r="M238" s="19"/>
@@ -8028,7 +8332,9 @@
         <v>1</v>
       </c>
       <c r="I239" s="19"/>
-      <c r="J239" s="19"/>
+      <c r="J239" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K239" s="19"/>
       <c r="L239" s="19"/>
       <c r="M239" s="19"/>
@@ -8054,7 +8360,9 @@
         <v>1</v>
       </c>
       <c r="I240" s="19"/>
-      <c r="J240" s="19"/>
+      <c r="J240" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="K240" s="19"/>
       <c r="L240" s="19"/>
       <c r="M240" s="19"/>
@@ -8080,7 +8388,9 @@
         <v>1</v>
       </c>
       <c r="I241" s="19"/>
-      <c r="J241" s="19"/>
+      <c r="J241" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K241" s="19"/>
       <c r="L241" s="19"/>
       <c r="M241" s="19"/>
@@ -8106,7 +8416,9 @@
         <v>1</v>
       </c>
       <c r="I242" s="19"/>
-      <c r="J242" s="19"/>
+      <c r="J242" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="K242" s="19"/>
       <c r="L242" s="19"/>
       <c r="M242" s="19"/>

</xml_diff>